<commit_message>
fixed snps and gene content tables
</commit_message>
<xml_diff>
--- a/data/snps_gene_content.xlsx
+++ b/data/snps_gene_content.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesliekollar/Desktop/Mimulus_genome_assembly/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA64EC8-89F4-8049-8765-3C196AE9FF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20925F72-C991-594F-B1C3-A70129E7F7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="15440" xr2:uid="{4367C880-65DC-9A41-851E-D25741B40FB0}"/>
+    <workbookView xWindow="320" yWindow="500" windowWidth="26840" windowHeight="15440" xr2:uid="{4367C880-65DC-9A41-851E-D25741B40FB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Genome wide</t>
   </si>
@@ -96,13 +96,16 @@
   </si>
   <si>
     <t>S1</t>
+  </si>
+  <si>
+    <t>Genome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +127,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,68 +475,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E35B6FF-098A-8D43-A03F-D67F0C69EDD7}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>176622</v>
       </c>
       <c r="C3">
-        <v>41</v>
-      </c>
-      <c r="D3" s="2">
-        <v>802</v>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>42</v>
       </c>
       <c r="E3">
-        <v>761</v>
+        <v>795</v>
       </c>
       <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F3:F14" si="0">(E3-D3)</f>
+        <v>753</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -543,235 +561,283 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6553</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>202</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>173</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>2787</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="E6">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>7299</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>211</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>6359</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>196</v>
+        <v>11</v>
       </c>
       <c r="E8">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>166</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>7002</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>12</v>
       </c>
-      <c r="D9">
-        <v>195</v>
-      </c>
       <c r="E9">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>723</v>
       </c>
       <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>4</v>
       </c>
-      <c r="D10">
-        <v>35</v>
-      </c>
       <c r="E10">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>206676</v>
       </c>
       <c r="C11">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>625</v>
+        <v>36</v>
       </c>
       <c r="E11">
-        <v>588</v>
+        <v>611</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>575</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>24553</v>
       </c>
       <c r="C12">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>318</v>
+        <v>18</v>
       </c>
       <c r="E12">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>23299</v>
       </c>
       <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>20</v>
       </c>
-      <c r="D13">
-        <v>261</v>
-      </c>
       <c r="E13">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>233</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>3986</v>
       </c>
       <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
         <v>9</v>
       </c>
-      <c r="D14">
-        <v>146</v>
-      </c>
       <c r="E14">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>177538</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>745</v>
       </c>
       <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <f>(E16-D16)</f>
+        <v>701</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -788,209 +854,254 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F17:F27" si="1">(E17-D17)</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>6531</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>184</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>2638</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>7541</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>6393</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>168</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>6951</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>159</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>18329</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>584</v>
       </c>
       <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>548</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>24882</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>291</v>
       </c>
       <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>274</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>22595</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>235</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>4109</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>